<commit_message>
JAMO update up to SDR-780 (from the bottom)
JAMO update up to SDR-780 (from the bottom)
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 09_15_2019/Offsets and Clip times 09_15_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 09_15_2019/Offsets and Clip times 09_15_2019.xlsx
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Clips!$A$1:$F$503</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Offsets!$A$1:$H$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Offsets!$A$1:$H$58</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="143">
   <si>
     <t>Site</t>
   </si>
@@ -363,12 +363,6 @@
     <t>Appears to be bad data.</t>
   </si>
   <si>
-    <t>Debris</t>
-  </si>
-  <si>
-    <t>Removed since this raised flow was noticebly higher than surrounding high flows.</t>
-  </si>
-  <si>
     <t>Obstruction in weir-confirmed by gamecam</t>
   </si>
   <si>
@@ -445,6 +439,27 @@
   </si>
   <si>
     <t>Weird red color 7/30. A series of wet weather events in May. Confirmed pool overflow 6/13-6/21 and 7/20-7/22. Field staff noted on 7/31 that SLR-045 level was lower than SLR-045A. Field staff suspected leak and added extra morter around weir seam. From 7/28 on, consistent negative level periods in raw data. Data processing team suspects a leak in the conveyance between SLR-045A and SLR-045B.</t>
+  </si>
+  <si>
+    <t>Appears to have drifted after May ww events</t>
+  </si>
+  <si>
+    <t>Appears to have drifted after sept ww event</t>
+  </si>
+  <si>
+    <t>Jn</t>
+  </si>
+  <si>
+    <t>A series of wet weather events in May. Two wet weather events in June.  Last wet weather event 9/4. Applied offsets due to apparent drifting caused by May and September ww events</t>
+  </si>
+  <si>
+    <t>added on 9/15 deliverable</t>
+  </si>
+  <si>
+    <t>modified old clip by LD. Revision added added on 9/15 deliverable</t>
+  </si>
+  <si>
+    <t>A series of wet weather events in May and one in september. Several high flow events not assosiated with wet weather (5/13-5/14, 8/15, and 9/13). Applied 0.2" offset to entire data set to improve calibration.</t>
   </si>
 </sst>
 </file>
@@ -958,10 +973,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +1013,7 @@
         <v>52</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1242,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>63</v>
@@ -1733,18 +1748,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="6"/>
+      <c r="E41" s="18">
+        <v>0.2</v>
+      </c>
       <c r="F41" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1761,7 +1779,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>44</v>
       </c>
@@ -2020,11 +2038,57 @@
         <v>65</v>
       </c>
     </row>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="1">
+        <v>43612.197916666664</v>
+      </c>
+      <c r="C57" s="7">
+        <v>43712.701388888891</v>
+      </c>
+      <c r="D57">
+        <v>-0.3</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G57" t="s">
+        <v>136</v>
+      </c>
+      <c r="H57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B58" s="7">
+        <v>43712.704861111109</v>
+      </c>
+      <c r="C58" s="1">
+        <v>43723.996527777781</v>
+      </c>
+      <c r="D58">
+        <v>-0.6</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H58" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H56">
+  <autoFilter ref="A1:H58">
     <filterColumn colId="0">
       <filters>
-        <filter val="SLR-045"/>
+        <filter val="SDR-780"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2040,11 +2104,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F503"/>
+  <dimension ref="A1:F506"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E423" sqref="E423"/>
+      <selection pane="bottomLeft" activeCell="A391" sqref="A391:XFD391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,7 +2116,7 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="25.7109375" style="7" customWidth="1"/>
     <col min="4" max="4" width="56.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2072,7 +2136,7 @@
         <v>52</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2509,7 +2573,7 @@
         <v>43647.618055555555</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>63</v>
@@ -3010,7 +3074,7 @@
         <v>43707.704861111109</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>63</v>
@@ -6945,7 +7009,7 @@
         <v>43691.541666666664</v>
       </c>
       <c r="D282" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F282" s="6" t="s">
         <v>63</v>
@@ -8815,130 +8879,137 @@
         <v>90</v>
       </c>
     </row>
-    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B389" s="7">
-        <v>43594.114583333336</v>
+        <v>43593.857638888891</v>
       </c>
       <c r="C389" s="7">
-        <v>43594.291666666664</v>
+        <v>43594.041666666664</v>
       </c>
       <c r="D389" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E389" s="6"/>
+      <c r="E389" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="F389" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B390" s="7">
-        <v>43596.541666666664</v>
+        <v>43596.319444444445</v>
       </c>
       <c r="C390" s="7">
-        <v>43597.083333333336</v>
+        <v>43596.704861111109</v>
       </c>
       <c r="D390" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E390" s="6"/>
+      <c r="E390" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="F390" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A391" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A391" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B391" s="7">
-        <v>43633.333333333336</v>
-      </c>
-      <c r="C391" s="7">
-        <v>43633.833333333336</v>
-      </c>
-      <c r="D391" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E391" s="6"/>
-      <c r="F391" s="6" t="s">
+      <c r="B391" s="14">
+        <v>43641.416666666664</v>
+      </c>
+      <c r="C391" s="14">
+        <v>43641.427083333336</v>
+      </c>
+      <c r="D391" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F391" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B392" s="7">
-        <v>43641.416666666664</v>
+        <v>43601.409722222219</v>
       </c>
       <c r="C392" s="7">
-        <v>43641.427083333336</v>
+        <v>43601.628472222219</v>
       </c>
       <c r="D392" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E392" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="E392" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="F392" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B393" s="7">
-        <v>43645</v>
+        <v>43604.416666666664</v>
       </c>
       <c r="C393" s="7">
-        <v>43645.1875</v>
+        <v>43605.694444444445</v>
       </c>
       <c r="D393" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E393" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="E393" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="F393" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B394" s="7">
-        <v>43645.229166666664</v>
+        <v>43607.180555555555</v>
       </c>
       <c r="C394" s="7">
-        <v>43645.395833333336</v>
+        <v>43608.427083333336</v>
       </c>
       <c r="D394" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E394" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="E394" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="F394" s="6" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B395" s="7">
-        <v>43660.770833333336</v>
+        <v>43591.583333333336</v>
       </c>
       <c r="C395" s="7">
-        <v>43661.513888888891</v>
+        <v>43592.041666666664</v>
       </c>
       <c r="D395" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E395" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E395" s="6"/>
       <c r="F395" s="6" t="s">
         <v>56</v>
       </c>
@@ -8948,10 +9019,10 @@
         <v>39</v>
       </c>
       <c r="B396" s="7">
-        <v>43591.583333333336</v>
+        <v>43592.427083333336</v>
       </c>
       <c r="C396" s="7">
-        <v>43592.041666666664</v>
+        <v>43593.125</v>
       </c>
       <c r="D396" s="6" t="s">
         <v>47</v>
@@ -8966,10 +9037,10 @@
         <v>39</v>
       </c>
       <c r="B397" s="7">
-        <v>43592.427083333336</v>
+        <v>43593.958333333336</v>
       </c>
       <c r="C397" s="7">
-        <v>43593.125</v>
+        <v>43594.375</v>
       </c>
       <c r="D397" s="6" t="s">
         <v>47</v>
@@ -8984,10 +9055,10 @@
         <v>39</v>
       </c>
       <c r="B398" s="7">
-        <v>43593.958333333336</v>
+        <v>43594.833333333336</v>
       </c>
       <c r="C398" s="7">
-        <v>43594.375</v>
+        <v>43595.3125</v>
       </c>
       <c r="D398" s="6" t="s">
         <v>47</v>
@@ -9002,10 +9073,10 @@
         <v>39</v>
       </c>
       <c r="B399" s="7">
-        <v>43594.833333333336</v>
+        <v>43596.541666666664</v>
       </c>
       <c r="C399" s="7">
-        <v>43595.3125</v>
+        <v>43597.291666666664</v>
       </c>
       <c r="D399" s="6" t="s">
         <v>47</v>
@@ -9017,49 +9088,49 @@
     </row>
     <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B400" s="7">
-        <v>43596.541666666664</v>
+        <v>43586</v>
       </c>
       <c r="C400" s="7">
-        <v>43597.291666666664</v>
+        <v>43586.847222222219</v>
       </c>
       <c r="D400" s="6" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="E400" s="6"/>
       <c r="F400" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B401" s="7">
-        <v>43586</v>
+        <v>43591.375</v>
       </c>
       <c r="C401" s="7">
-        <v>43586.847222222219</v>
+        <v>43591.458333333336</v>
       </c>
       <c r="D401" s="6" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="E401" s="6"/>
       <c r="F401" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B402" s="7">
-        <v>43591.375</v>
+        <v>43596.291666666664</v>
       </c>
       <c r="C402" s="7">
-        <v>43591.458333333336</v>
+        <v>43596.458333333336</v>
       </c>
       <c r="D402" s="6" t="s">
         <v>47</v>
@@ -9069,53 +9140,53 @@
         <v>63</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B403" s="7">
-        <v>43596.291666666664</v>
+        <v>43601.333333333336</v>
       </c>
       <c r="C403" s="7">
-        <v>43596.458333333336</v>
+        <v>43601.583333333336</v>
       </c>
       <c r="D403" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E403" s="6"/>
+      <c r="E403" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="F403" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B404" s="7">
-        <v>43601.333333333336</v>
+        <v>43604.291666666664</v>
       </c>
       <c r="C404" s="7">
-        <v>43601.583333333336</v>
+        <v>43605.583333333336</v>
       </c>
       <c r="D404" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E404" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="E404" s="6"/>
       <c r="F404" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B405" s="7">
-        <v>43604.291666666664</v>
+        <v>43607.25</v>
       </c>
       <c r="C405" s="7">
-        <v>43605.583333333336</v>
+        <v>43607.541666666664</v>
       </c>
       <c r="D405" s="6" t="s">
         <v>47</v>
@@ -9125,15 +9196,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B406" s="7">
-        <v>43607.25</v>
+        <v>43611.291666666664</v>
       </c>
       <c r="C406" s="7">
-        <v>43607.541666666664</v>
+        <v>43613</v>
       </c>
       <c r="D406" s="6" t="s">
         <v>47</v>
@@ -9143,33 +9214,33 @@
         <v>63</v>
       </c>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B407" s="7">
-        <v>43611.291666666664</v>
+        <v>43633.166666666664</v>
       </c>
       <c r="C407" s="7">
-        <v>43613</v>
+        <v>43633.458333333336</v>
       </c>
       <c r="D407" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E407" s="6"/>
       <c r="F407" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B408" s="7">
-        <v>43633.166666666664</v>
+        <v>43637.270833333336</v>
       </c>
       <c r="C408" s="7">
-        <v>43633.458333333336</v>
+        <v>43637.416666666664</v>
       </c>
       <c r="D408" s="6" t="s">
         <v>47</v>
@@ -9179,71 +9250,73 @@
         <v>90</v>
       </c>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A409" s="3" t="s">
+    <row r="409" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A409" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B409" s="7">
-        <v>43637.270833333336</v>
+        <v>43654.288194444445</v>
       </c>
       <c r="C409" s="7">
-        <v>43637.416666666664</v>
+        <v>43654.788194444445</v>
       </c>
       <c r="D409" s="6" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="E409" s="6"/>
       <c r="F409" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B410" s="7">
-        <v>43654.288194444445</v>
+        <v>43691.427083333336</v>
       </c>
       <c r="C410" s="7">
-        <v>43654.788194444445</v>
+        <v>43692.385416666664</v>
       </c>
       <c r="D410" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E410" s="6"/>
+        <v>126</v>
+      </c>
       <c r="F410" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="411" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B411" s="7">
-        <v>43691.427083333336</v>
+        <v>43684.361111111109</v>
       </c>
       <c r="C411" s="7">
-        <v>43692.385416666664</v>
+        <v>43685.361111111109</v>
       </c>
       <c r="D411" s="6" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F411" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="412" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A412" s="7" t="s">
-        <v>44</v>
+    <row r="412" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A412" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B412" s="7">
-        <v>43684.361111111109</v>
+        <v>43586</v>
       </c>
       <c r="C412" s="7">
-        <v>43685.361111111109</v>
+        <v>43586.572916666664</v>
       </c>
       <c r="D412" s="6" t="s">
-        <v>112</v>
+        <v>86</v>
+      </c>
+      <c r="E412" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="F412" s="6" t="s">
         <v>63</v>
@@ -9254,17 +9327,15 @@
         <v>45</v>
       </c>
       <c r="B413" s="7">
-        <v>43586</v>
+        <v>43591.375</v>
       </c>
       <c r="C413" s="7">
-        <v>43586.572916666664</v>
+        <v>43591.458333333336</v>
       </c>
       <c r="D413" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E413" s="6" t="s">
-        <v>51</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E413" s="6"/>
       <c r="F413" s="6" t="s">
         <v>63</v>
       </c>
@@ -9274,13 +9345,13 @@
         <v>45</v>
       </c>
       <c r="B414" s="7">
-        <v>43591.375</v>
+        <v>43594.875</v>
       </c>
       <c r="C414" s="7">
-        <v>43591.458333333336</v>
+        <v>43595.708333333336</v>
       </c>
       <c r="D414" s="6" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E414" s="6"/>
       <c r="F414" s="6" t="s">
@@ -9292,13 +9363,13 @@
         <v>45</v>
       </c>
       <c r="B415" s="7">
-        <v>43594.875</v>
+        <v>43596.291666666664</v>
       </c>
       <c r="C415" s="7">
-        <v>43595.708333333336</v>
+        <v>43596.458333333336</v>
       </c>
       <c r="D415" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E415" s="6"/>
       <c r="F415" s="6" t="s">
@@ -9310,13 +9381,13 @@
         <v>45</v>
       </c>
       <c r="B416" s="7">
-        <v>43596.291666666664</v>
+        <v>43598</v>
       </c>
       <c r="C416" s="7">
-        <v>43596.458333333336</v>
+        <v>43598.697916666664</v>
       </c>
       <c r="D416" s="6" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E416" s="6"/>
       <c r="F416" s="6" t="s">
@@ -9328,10 +9399,10 @@
         <v>45</v>
       </c>
       <c r="B417" s="7">
-        <v>43598</v>
+        <v>43599.479166666664</v>
       </c>
       <c r="C417" s="7">
-        <v>43598.697916666664</v>
+        <v>43600.114583333336</v>
       </c>
       <c r="D417" s="6" t="s">
         <v>59</v>
@@ -9346,13 +9417,13 @@
         <v>45</v>
       </c>
       <c r="B418" s="7">
-        <v>43599.479166666664</v>
+        <v>43601.333333333336</v>
       </c>
       <c r="C418" s="7">
-        <v>43600.114583333336</v>
+        <v>43601.583333333336</v>
       </c>
       <c r="D418" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E418" s="6"/>
       <c r="F418" s="6" t="s">
@@ -9364,10 +9435,10 @@
         <v>45</v>
       </c>
       <c r="B419" s="7">
-        <v>43601.333333333336</v>
+        <v>43604.291666666664</v>
       </c>
       <c r="C419" s="7">
-        <v>43601.583333333336</v>
+        <v>43605.583333333336</v>
       </c>
       <c r="D419" s="6" t="s">
         <v>47</v>
@@ -9382,10 +9453,10 @@
         <v>45</v>
       </c>
       <c r="B420" s="7">
-        <v>43604.291666666664</v>
+        <v>43607.25</v>
       </c>
       <c r="C420" s="7">
-        <v>43605.583333333336</v>
+        <v>43607.541666666664</v>
       </c>
       <c r="D420" s="6" t="s">
         <v>47</v>
@@ -9400,10 +9471,10 @@
         <v>45</v>
       </c>
       <c r="B421" s="7">
-        <v>43607.25</v>
+        <v>43611.291666666664</v>
       </c>
       <c r="C421" s="7">
-        <v>43607.541666666664</v>
+        <v>43613</v>
       </c>
       <c r="D421" s="6" t="s">
         <v>47</v>
@@ -9418,17 +9489,19 @@
         <v>45</v>
       </c>
       <c r="B422" s="7">
-        <v>43611.291666666664</v>
+        <v>43655.552083333336</v>
       </c>
       <c r="C422" s="7">
-        <v>43613</v>
+        <v>43661.5625</v>
       </c>
       <c r="D422" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E422" s="6"/>
+        <v>97</v>
+      </c>
+      <c r="E422" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="F422" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="423" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -9436,19 +9509,17 @@
         <v>45</v>
       </c>
       <c r="B423" s="7">
-        <v>43655.552083333336</v>
+        <v>43661.5625</v>
       </c>
       <c r="C423" s="7">
-        <v>43661.5625</v>
+        <v>43661.604166666664</v>
       </c>
       <c r="D423" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E423" s="6" t="s">
-        <v>98</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E423" s="6"/>
       <c r="F423" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="424" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -9462,25 +9533,25 @@
         <v>43661.604166666664</v>
       </c>
       <c r="D424" s="6" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="E424" s="6"/>
       <c r="F424" s="6" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="425" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A425" s="3" t="s">
+      <c r="A425" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B425" s="7">
-        <v>43661.5625</v>
+        <v>43668.784722222219</v>
       </c>
       <c r="C425" s="7">
-        <v>43661.604166666664</v>
+        <v>43669.243055555555</v>
       </c>
       <c r="D425" s="6" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="E425" s="6"/>
       <c r="F425" s="6" t="s">
@@ -9488,21 +9559,21 @@
       </c>
     </row>
     <row r="426" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A426" s="7" t="s">
-        <v>45</v>
+      <c r="A426" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B426" s="7">
-        <v>43668.784722222219</v>
+        <v>43619</v>
       </c>
       <c r="C426" s="7">
-        <v>43669.243055555555</v>
+        <v>43619.125</v>
       </c>
       <c r="D426" s="6" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E426" s="6"/>
       <c r="F426" s="6" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="427" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -9510,10 +9581,10 @@
         <v>46</v>
       </c>
       <c r="B427" s="7">
-        <v>43619</v>
+        <v>43633.083333333336</v>
       </c>
       <c r="C427" s="7">
-        <v>43619.125</v>
+        <v>43633.458333333336</v>
       </c>
       <c r="D427" s="6" t="s">
         <v>47</v>
@@ -9528,13 +9599,13 @@
         <v>46</v>
       </c>
       <c r="B428" s="7">
-        <v>43633.083333333336</v>
+        <v>43637</v>
       </c>
       <c r="C428" s="7">
-        <v>43633.458333333336</v>
+        <v>43641.541666666664</v>
       </c>
       <c r="D428" s="6" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="E428" s="6"/>
       <c r="F428" s="6" t="s">
@@ -9546,10 +9617,10 @@
         <v>46</v>
       </c>
       <c r="B429" s="7">
-        <v>43637</v>
+        <v>43643.291666666664</v>
       </c>
       <c r="C429" s="7">
-        <v>43641.541666666664</v>
+        <v>43643.666666666664</v>
       </c>
       <c r="D429" s="6" t="s">
         <v>89</v>
@@ -9564,10 +9635,10 @@
         <v>46</v>
       </c>
       <c r="B430" s="7">
-        <v>43643.291666666664</v>
+        <v>43644.229166666664</v>
       </c>
       <c r="C430" s="7">
-        <v>43643.666666666664</v>
+        <v>43644.583333333336</v>
       </c>
       <c r="D430" s="6" t="s">
         <v>89</v>
@@ -9582,10 +9653,10 @@
         <v>46</v>
       </c>
       <c r="B431" s="7">
-        <v>43644.229166666664</v>
+        <v>43645.21875</v>
       </c>
       <c r="C431" s="7">
-        <v>43644.583333333336</v>
+        <v>43645.5625</v>
       </c>
       <c r="D431" s="6" t="s">
         <v>89</v>
@@ -9599,33 +9670,33 @@
       <c r="A432" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B432" s="7">
-        <v>43645.21875</v>
-      </c>
-      <c r="C432" s="7">
-        <v>43645.5625</v>
-      </c>
-      <c r="D432" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E432" s="6"/>
+      <c r="B432" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D432" s="6"/>
+      <c r="E432" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="F432" s="6" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="433" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A433" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B433" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D433" s="6"/>
-      <c r="E433" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="A433" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B433" s="32">
+        <v>43591.375</v>
+      </c>
+      <c r="C433" s="32">
+        <v>43592.458333333336</v>
+      </c>
+      <c r="D433" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E433" s="6"/>
       <c r="F433" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="434" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -9633,13 +9704,13 @@
         <v>18</v>
       </c>
       <c r="B434" s="32">
-        <v>43591.375</v>
+        <v>43592.125</v>
       </c>
       <c r="C434" s="32">
-        <v>43592.458333333336</v>
+        <v>43594.416666666664</v>
       </c>
       <c r="D434" s="31" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="E434" s="6"/>
       <c r="F434" s="6" t="s">
@@ -9651,13 +9722,13 @@
         <v>18</v>
       </c>
       <c r="B435" s="32">
-        <v>43592.125</v>
+        <v>43595.291666666664</v>
       </c>
       <c r="C435" s="32">
-        <v>43594.416666666664</v>
+        <v>43595.416666666664</v>
       </c>
       <c r="D435" s="31" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="E435" s="6"/>
       <c r="F435" s="6" t="s">
@@ -9669,10 +9740,10 @@
         <v>18</v>
       </c>
       <c r="B436" s="32">
-        <v>43595.291666666664</v>
+        <v>43596.319444444445</v>
       </c>
       <c r="C436" s="32">
-        <v>43595.416666666664</v>
+        <v>43596.947916666664</v>
       </c>
       <c r="D436" s="31" t="s">
         <v>47</v>
@@ -9687,15 +9758,15 @@
         <v>18</v>
       </c>
       <c r="B437" s="32">
-        <v>43596.319444444445</v>
+        <v>43601.333333333336</v>
       </c>
       <c r="C437" s="32">
-        <v>43596.947916666664</v>
+        <v>43601.854166666664</v>
       </c>
       <c r="D437" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="E437" s="6"/>
+      <c r="E437" s="3"/>
       <c r="F437" s="6" t="s">
         <v>63</v>
       </c>
@@ -9705,15 +9776,15 @@
         <v>18</v>
       </c>
       <c r="B438" s="32">
-        <v>43601.333333333336</v>
+        <v>43604.083333333336</v>
       </c>
       <c r="C438" s="32">
-        <v>43601.854166666664</v>
+        <v>43605.1875</v>
       </c>
       <c r="D438" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="E438" s="3"/>
+      <c r="E438" s="6"/>
       <c r="F438" s="6" t="s">
         <v>63</v>
       </c>
@@ -9726,10 +9797,10 @@
         <v>43604.083333333336</v>
       </c>
       <c r="C439" s="32">
-        <v>43605.1875</v>
+        <v>43633.6875</v>
       </c>
       <c r="D439" s="31" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="E439" s="6"/>
       <c r="F439" s="6" t="s">
@@ -9741,17 +9812,17 @@
         <v>18</v>
       </c>
       <c r="B440" s="32">
-        <v>43604.083333333336</v>
+        <v>43637.270833333336</v>
       </c>
       <c r="C440" s="32">
-        <v>43633.6875</v>
+        <v>43637.479166666664</v>
       </c>
       <c r="D440" s="31" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="E440" s="6"/>
       <c r="F440" s="6" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
     </row>
     <row r="441" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -9759,67 +9830,67 @@
         <v>18</v>
       </c>
       <c r="B441" s="32">
-        <v>43637.270833333336</v>
+        <v>43663.302083333336</v>
       </c>
       <c r="C441" s="32">
-        <v>43637.479166666664</v>
+        <v>43665.5625</v>
       </c>
       <c r="D441" s="31" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="E441" s="6"/>
       <c r="F441" s="6" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="442" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A442" s="35" t="s">
+      <c r="A442" s="32" t="s">
         <v>18</v>
       </c>
       <c r="B442" s="32">
-        <v>43663.302083333336</v>
+        <v>43668.850694444445</v>
       </c>
       <c r="C442" s="32">
-        <v>43665.5625</v>
+        <v>43669.267361111109</v>
       </c>
       <c r="D442" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E442" s="6"/>
       <c r="F442" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="443" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="32" t="s">
         <v>18</v>
       </c>
       <c r="B443" s="32">
-        <v>43668.850694444445</v>
+        <v>43675.892361111109</v>
       </c>
       <c r="C443" s="32">
-        <v>43669.267361111109</v>
+        <v>43676.225694444445</v>
       </c>
       <c r="D443" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="E443" s="6"/>
-      <c r="F443" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="444" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A444" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B444" s="32">
-        <v>43675.892361111109</v>
-      </c>
-      <c r="C444" s="32">
-        <v>43676.225694444445</v>
-      </c>
-      <c r="D444" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A444" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B444" s="7">
+        <v>43575</v>
+      </c>
+      <c r="C444" s="7">
+        <v>43593.75</v>
+      </c>
+      <c r="D444" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E444" s="6"/>
+      <c r="F444" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="445" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -9827,13 +9898,13 @@
         <v>26</v>
       </c>
       <c r="B445" s="7">
-        <v>43575</v>
+        <v>43594.965277777781</v>
       </c>
       <c r="C445" s="7">
-        <v>43593.75</v>
+        <v>43595.375</v>
       </c>
       <c r="D445" s="6" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="E445" s="6"/>
       <c r="F445" s="6" t="s">
@@ -9845,10 +9916,10 @@
         <v>26</v>
       </c>
       <c r="B446" s="7">
-        <v>43594.965277777781</v>
+        <v>43596.395833333336</v>
       </c>
       <c r="C446" s="7">
-        <v>43595.375</v>
+        <v>43596.517361111109</v>
       </c>
       <c r="D446" s="6" t="s">
         <v>47</v>
@@ -9859,14 +9930,14 @@
       </c>
     </row>
     <row r="447" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A447" s="6" t="s">
+      <c r="A447" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B447" s="7">
-        <v>43596.395833333336</v>
+        <v>43601.420138888891</v>
       </c>
       <c r="C447" s="7">
-        <v>43596.517361111109</v>
+        <v>43601.604166666664</v>
       </c>
       <c r="D447" s="6" t="s">
         <v>47</v>
@@ -9881,10 +9952,10 @@
         <v>26</v>
       </c>
       <c r="B448" s="7">
-        <v>43601.420138888891</v>
+        <v>43604.4375</v>
       </c>
       <c r="C448" s="7">
-        <v>43601.604166666664</v>
+        <v>43604.638888888891</v>
       </c>
       <c r="D448" s="6" t="s">
         <v>47</v>
@@ -9899,10 +9970,10 @@
         <v>26</v>
       </c>
       <c r="B449" s="7">
-        <v>43604.4375</v>
+        <v>43604.875</v>
       </c>
       <c r="C449" s="7">
-        <v>43604.638888888891</v>
+        <v>43605.569444444445</v>
       </c>
       <c r="D449" s="6" t="s">
         <v>47</v>
@@ -9917,10 +9988,10 @@
         <v>26</v>
       </c>
       <c r="B450" s="7">
-        <v>43604.875</v>
+        <v>43607.239583333336</v>
       </c>
       <c r="C450" s="7">
-        <v>43605.569444444445</v>
+        <v>43607.354166666664</v>
       </c>
       <c r="D450" s="6" t="s">
         <v>47</v>
@@ -9934,11 +10005,11 @@
       <c r="A451" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B451" s="7">
-        <v>43607.239583333336</v>
-      </c>
-      <c r="C451" s="7">
-        <v>43607.354166666664</v>
+      <c r="B451" s="22">
+        <v>43611.885416666664</v>
+      </c>
+      <c r="C451" s="22">
+        <v>43612.34375</v>
       </c>
       <c r="D451" s="6" t="s">
         <v>47</v>
@@ -9953,10 +10024,10 @@
         <v>26</v>
       </c>
       <c r="B452" s="22">
-        <v>43611.885416666664</v>
+        <v>43637.208333333336</v>
       </c>
       <c r="C452" s="22">
-        <v>43612.34375</v>
+        <v>43637.416666666664</v>
       </c>
       <c r="D452" s="6" t="s">
         <v>47</v>
@@ -9967,14 +10038,14 @@
       </c>
     </row>
     <row r="453" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A453" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B453" s="22">
-        <v>43637.208333333336</v>
-      </c>
-      <c r="C453" s="22">
-        <v>43637.416666666664</v>
+      <c r="A453" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B453" s="7">
+        <v>43591.333333333336</v>
+      </c>
+      <c r="C453" s="7">
+        <v>43591.479166666664</v>
       </c>
       <c r="D453" s="6" t="s">
         <v>47</v>
@@ -9989,10 +10060,10 @@
         <v>19</v>
       </c>
       <c r="B454" s="7">
-        <v>43591.333333333336</v>
+        <v>43592.173611111109</v>
       </c>
       <c r="C454" s="7">
-        <v>43591.479166666664</v>
+        <v>43592.288194444445</v>
       </c>
       <c r="D454" s="6" t="s">
         <v>47</v>
@@ -10007,10 +10078,10 @@
         <v>19</v>
       </c>
       <c r="B455" s="7">
-        <v>43592.173611111109</v>
+        <v>43595.041666666664</v>
       </c>
       <c r="C455" s="7">
-        <v>43592.288194444445</v>
+        <v>43595.322916666664</v>
       </c>
       <c r="D455" s="6" t="s">
         <v>47</v>
@@ -10025,10 +10096,10 @@
         <v>19</v>
       </c>
       <c r="B456" s="7">
-        <v>43595.041666666664</v>
+        <v>43596.270833333336</v>
       </c>
       <c r="C456" s="7">
-        <v>43595.322916666664</v>
+        <v>43596.534722222219</v>
       </c>
       <c r="D456" s="6" t="s">
         <v>47</v>
@@ -10043,10 +10114,10 @@
         <v>19</v>
       </c>
       <c r="B457" s="7">
-        <v>43596.270833333336</v>
+        <v>43601.40625</v>
       </c>
       <c r="C457" s="7">
-        <v>43596.534722222219</v>
+        <v>43601.565972222219</v>
       </c>
       <c r="D457" s="6" t="s">
         <v>47</v>
@@ -10061,10 +10132,10 @@
         <v>19</v>
       </c>
       <c r="B458" s="7">
-        <v>43601.40625</v>
+        <v>43604.416666666664</v>
       </c>
       <c r="C458" s="7">
-        <v>43601.565972222219</v>
+        <v>43605.368055555555</v>
       </c>
       <c r="D458" s="6" t="s">
         <v>47</v>
@@ -10079,10 +10150,10 @@
         <v>19</v>
       </c>
       <c r="B459" s="7">
-        <v>43604.416666666664</v>
+        <v>43606.951388888891</v>
       </c>
       <c r="C459" s="7">
-        <v>43605.368055555555</v>
+        <v>43607.875</v>
       </c>
       <c r="D459" s="6" t="s">
         <v>47</v>
@@ -10097,10 +10168,10 @@
         <v>19</v>
       </c>
       <c r="B460" s="7">
-        <v>43606.951388888891</v>
+        <v>43611.9375</v>
       </c>
       <c r="C460" s="7">
-        <v>43607.875</v>
+        <v>43612.111111111109</v>
       </c>
       <c r="D460" s="6" t="s">
         <v>47</v>
@@ -10111,22 +10182,10 @@
       </c>
     </row>
     <row r="461" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A461" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B461" s="7">
-        <v>43611.9375</v>
-      </c>
-      <c r="C461" s="7">
-        <v>43612.111111111109</v>
-      </c>
-      <c r="D461" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="A461" s="6"/>
+      <c r="D461" s="6"/>
       <c r="E461" s="6"/>
-      <c r="F461" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="F461" s="6"/>
     </row>
     <row r="462" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" s="6"/>
@@ -10171,20 +10230,32 @@
       <c r="F468" s="6"/>
     </row>
     <row r="469" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A469" s="6"/>
-      <c r="D469" s="6"/>
+      <c r="A469" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B469" s="7">
+        <v>43591.409722222219</v>
+      </c>
+      <c r="C469" s="7">
+        <v>43592.583333333336</v>
+      </c>
+      <c r="D469" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="E469" s="6"/>
-      <c r="F469" s="6"/>
+      <c r="F469" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="470" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B470" s="7">
-        <v>43591.409722222219</v>
+        <v>43595.194444444445</v>
       </c>
       <c r="C470" s="7">
-        <v>43592.583333333336</v>
+        <v>43595.4375</v>
       </c>
       <c r="D470" s="6" t="s">
         <v>47</v>
@@ -10199,10 +10270,10 @@
         <v>20</v>
       </c>
       <c r="B471" s="7">
-        <v>43595.194444444445</v>
+        <v>43595.260416666664</v>
       </c>
       <c r="C471" s="7">
-        <v>43595.4375</v>
+        <v>43594.875</v>
       </c>
       <c r="D471" s="6" t="s">
         <v>47</v>
@@ -10217,10 +10288,10 @@
         <v>20</v>
       </c>
       <c r="B472" s="7">
-        <v>43595.260416666664</v>
+        <v>43596.340277777781</v>
       </c>
       <c r="C472" s="7">
-        <v>43594.875</v>
+        <v>43596.895833333336</v>
       </c>
       <c r="D472" s="6" t="s">
         <v>47</v>
@@ -10235,10 +10306,10 @@
         <v>20</v>
       </c>
       <c r="B473" s="7">
-        <v>43596.340277777781</v>
+        <v>43601.440972222219</v>
       </c>
       <c r="C473" s="7">
-        <v>43596.895833333336</v>
+        <v>43601.822916666664</v>
       </c>
       <c r="D473" s="6" t="s">
         <v>47</v>
@@ -10253,10 +10324,10 @@
         <v>20</v>
       </c>
       <c r="B474" s="7">
-        <v>43601.440972222219</v>
+        <v>43604.440972222219</v>
       </c>
       <c r="C474" s="7">
-        <v>43601.822916666664</v>
+        <v>43608.708333333336</v>
       </c>
       <c r="D474" s="6" t="s">
         <v>47</v>
@@ -10271,10 +10342,10 @@
         <v>20</v>
       </c>
       <c r="B475" s="7">
-        <v>43604.440972222219</v>
+        <v>43610.291666666664</v>
       </c>
       <c r="C475" s="7">
-        <v>43608.708333333336</v>
+        <v>43612.25</v>
       </c>
       <c r="D475" s="6" t="s">
         <v>47</v>
@@ -10289,17 +10360,17 @@
         <v>20</v>
       </c>
       <c r="B476" s="7">
-        <v>43610.291666666664</v>
+        <v>43633.583333333336</v>
       </c>
       <c r="C476" s="7">
-        <v>43612.25</v>
+        <v>43633.833333333336</v>
       </c>
       <c r="D476" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E476" s="6"/>
       <c r="F476" s="6" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
     </row>
     <row r="477" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -10307,10 +10378,10 @@
         <v>20</v>
       </c>
       <c r="B477" s="7">
-        <v>43633.583333333336</v>
+        <v>43637.104166666664</v>
       </c>
       <c r="C477" s="7">
-        <v>43633.833333333336</v>
+        <v>43637.791666666664</v>
       </c>
       <c r="D477" s="6" t="s">
         <v>47</v>
@@ -10325,13 +10396,13 @@
         <v>20</v>
       </c>
       <c r="B478" s="7">
-        <v>43637.104166666664</v>
+        <v>43646</v>
       </c>
       <c r="C478" s="7">
-        <v>43637.791666666664</v>
+        <v>43646.020833333336</v>
       </c>
       <c r="D478" s="6" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="E478" s="6"/>
       <c r="F478" s="6" t="s">
@@ -10343,17 +10414,17 @@
         <v>20</v>
       </c>
       <c r="B479" s="7">
-        <v>43646</v>
+        <v>43647.392361111109</v>
       </c>
       <c r="C479" s="7">
-        <v>43646.020833333336</v>
+        <v>43647.559027777781</v>
       </c>
       <c r="D479" s="6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E479" s="6"/>
       <c r="F479" s="6" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
     </row>
     <row r="480" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -10361,10 +10432,10 @@
         <v>20</v>
       </c>
       <c r="B480" s="7">
-        <v>43647.392361111109</v>
+        <v>43649.385416666664</v>
       </c>
       <c r="C480" s="7">
-        <v>43647.559027777781</v>
+        <v>43649.552083333336</v>
       </c>
       <c r="D480" s="6" t="s">
         <v>78</v>
@@ -10379,10 +10450,10 @@
         <v>20</v>
       </c>
       <c r="B481" s="7">
-        <v>43649.385416666664</v>
+        <v>43655.010416666664</v>
       </c>
       <c r="C481" s="7">
-        <v>43649.552083333336</v>
+        <v>43655.177083333336</v>
       </c>
       <c r="D481" s="6" t="s">
         <v>78</v>
@@ -10397,10 +10468,10 @@
         <v>20</v>
       </c>
       <c r="B482" s="7">
-        <v>43655.010416666664</v>
+        <v>43665.013888888891</v>
       </c>
       <c r="C482" s="7">
-        <v>43655.177083333336</v>
+        <v>43665.180555555555</v>
       </c>
       <c r="D482" s="6" t="s">
         <v>78</v>
@@ -10415,10 +10486,10 @@
         <v>20</v>
       </c>
       <c r="B483" s="7">
-        <v>43665.013888888891</v>
+        <v>43666.013888888891</v>
       </c>
       <c r="C483" s="7">
-        <v>43665.180555555555</v>
+        <v>43666.180555555555</v>
       </c>
       <c r="D483" s="6" t="s">
         <v>78</v>
@@ -10433,10 +10504,10 @@
         <v>20</v>
       </c>
       <c r="B484" s="7">
-        <v>43666.013888888891</v>
+        <v>43668.010416666664</v>
       </c>
       <c r="C484" s="7">
-        <v>43666.180555555555</v>
+        <v>43668.177083333336</v>
       </c>
       <c r="D484" s="6" t="s">
         <v>78</v>
@@ -10451,10 +10522,10 @@
         <v>20</v>
       </c>
       <c r="B485" s="7">
-        <v>43668.010416666664</v>
+        <v>43669</v>
       </c>
       <c r="C485" s="7">
-        <v>43668.177083333336</v>
+        <v>43669.006944444445</v>
       </c>
       <c r="D485" s="6" t="s">
         <v>78</v>
@@ -10469,10 +10540,10 @@
         <v>20</v>
       </c>
       <c r="B486" s="7">
-        <v>43669</v>
+        <v>43670</v>
       </c>
       <c r="C486" s="7">
-        <v>43669.006944444445</v>
+        <v>43670.006944444445</v>
       </c>
       <c r="D486" s="6" t="s">
         <v>78</v>
@@ -10487,10 +10558,10 @@
         <v>20</v>
       </c>
       <c r="B487" s="7">
-        <v>43670</v>
+        <v>43670.545138888891</v>
       </c>
       <c r="C487" s="7">
-        <v>43670.006944444445</v>
+        <v>43670.711805555555</v>
       </c>
       <c r="D487" s="6" t="s">
         <v>78</v>
@@ -10502,20 +10573,20 @@
     </row>
     <row r="488" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B488" s="7">
-        <v>43670.545138888891</v>
+        <v>43591.375</v>
       </c>
       <c r="C488" s="7">
-        <v>43670.711805555555</v>
+        <v>43591.78125</v>
       </c>
       <c r="D488" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="E488" s="6"/>
       <c r="F488" s="6" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="489" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -10523,10 +10594,10 @@
         <v>25</v>
       </c>
       <c r="B489" s="7">
-        <v>43591.375</v>
+        <v>43592.166666666664</v>
       </c>
       <c r="C489" s="7">
-        <v>43591.78125</v>
+        <v>43592.579861111109</v>
       </c>
       <c r="D489" s="6" t="s">
         <v>47</v>
@@ -10541,16 +10612,15 @@
         <v>25</v>
       </c>
       <c r="B490" s="7">
-        <v>43592.166666666664</v>
+        <v>43595.194444444445</v>
       </c>
       <c r="C490" s="7">
-        <v>43592.579861111109</v>
+        <v>43595.4375</v>
       </c>
       <c r="D490" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E490" s="6"/>
-      <c r="F490" s="6" t="s">
+      <c r="F490" t="s">
         <v>63</v>
       </c>
     </row>
@@ -10559,15 +10629,15 @@
         <v>25</v>
       </c>
       <c r="B491" s="7">
-        <v>43595.194444444445</v>
+        <v>43595.260416666664</v>
       </c>
       <c r="C491" s="7">
-        <v>43595.4375</v>
+        <v>43594.875</v>
       </c>
       <c r="D491" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F491" t="s">
+      <c r="F491" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -10576,10 +10646,10 @@
         <v>25</v>
       </c>
       <c r="B492" s="7">
-        <v>43595.260416666664</v>
+        <v>43596.340277777781</v>
       </c>
       <c r="C492" s="7">
-        <v>43594.875</v>
+        <v>43596.895833333336</v>
       </c>
       <c r="D492" s="6" t="s">
         <v>47</v>
@@ -10593,15 +10663,15 @@
         <v>25</v>
       </c>
       <c r="B493" s="7">
-        <v>43596.340277777781</v>
+        <v>43601.388888888891</v>
       </c>
       <c r="C493" s="7">
-        <v>43596.895833333336</v>
+        <v>43601.822916666664</v>
       </c>
       <c r="D493" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F493" s="6" t="s">
+      <c r="F493" t="s">
         <v>63</v>
       </c>
     </row>
@@ -10610,14 +10680,15 @@
         <v>25</v>
       </c>
       <c r="B494" s="7">
-        <v>43601.388888888891</v>
+        <v>43604.350694444445</v>
       </c>
       <c r="C494" s="7">
-        <v>43601.822916666664</v>
+        <v>43608.708333333336</v>
       </c>
       <c r="D494" s="6" t="s">
         <v>47</v>
       </c>
+      <c r="E494" s="6"/>
       <c r="F494" t="s">
         <v>63</v>
       </c>
@@ -10627,16 +10698,16 @@
         <v>25</v>
       </c>
       <c r="B495" s="7">
-        <v>43604.350694444445</v>
+        <v>43611.892361111109</v>
       </c>
       <c r="C495" s="7">
-        <v>43608.708333333336</v>
+        <v>43612.25</v>
       </c>
       <c r="D495" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E495" s="6"/>
-      <c r="F495" t="s">
+      <c r="F495" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -10645,13 +10716,13 @@
         <v>25</v>
       </c>
       <c r="B496" s="7">
-        <v>43611.892361111109</v>
+        <v>43616.208333333336</v>
       </c>
       <c r="C496" s="7">
-        <v>43612.25</v>
+        <v>43616.701388888891</v>
       </c>
       <c r="D496" s="6" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E496" s="6"/>
       <c r="F496" s="6" t="s">
@@ -10663,17 +10734,17 @@
         <v>25</v>
       </c>
       <c r="B497" s="7">
-        <v>43616.208333333336</v>
+        <v>43633.583333333336</v>
       </c>
       <c r="C497" s="7">
-        <v>43616.701388888891</v>
+        <v>43633.791666666664</v>
       </c>
       <c r="D497" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E497" s="6"/>
-      <c r="F497" s="6" t="s">
-        <v>63</v>
+      <c r="F497" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="498" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -10681,10 +10752,10 @@
         <v>25</v>
       </c>
       <c r="B498" s="7">
-        <v>43633.583333333336</v>
+        <v>43637.104166666664</v>
       </c>
       <c r="C498" s="7">
-        <v>43633.791666666664</v>
+        <v>43637.791666666664</v>
       </c>
       <c r="D498" s="6" t="s">
         <v>47</v>
@@ -10695,26 +10766,25 @@
       </c>
     </row>
     <row r="499" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A499" s="6" t="s">
+      <c r="A499" t="s">
         <v>25</v>
       </c>
       <c r="B499" s="7">
-        <v>43637.104166666664</v>
+        <v>43712.618055555555</v>
       </c>
       <c r="C499" s="7">
-        <v>43637.791666666664</v>
-      </c>
-      <c r="D499" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E499" s="6"/>
+        <v>43712.847222222219</v>
+      </c>
+      <c r="D499" t="s">
+        <v>47</v>
+      </c>
       <c r="F499" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="500" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B500" s="7">
         <v>43712.618055555555</v>
@@ -10722,16 +10792,16 @@
       <c r="C500" s="7">
         <v>43712.847222222219</v>
       </c>
-      <c r="D500" t="s">
-        <v>47</v>
-      </c>
-      <c r="F500" t="s">
+      <c r="D500" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F500" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="501" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B501" s="7">
         <v>43712.618055555555</v>
@@ -10742,42 +10812,102 @@
       <c r="D501" s="6" t="s">
         <v>47</v>
       </c>
+      <c r="E501" s="6"/>
       <c r="F501" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="502" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B502" s="7">
-        <v>43712.618055555555</v>
+        <v>43712.625</v>
       </c>
       <c r="C502" s="7">
-        <v>43712.847222222219</v>
+        <v>43712.673611111109</v>
       </c>
       <c r="D502" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E502" s="6"/>
       <c r="F502" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="503" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A503" t="s">
-        <v>26</v>
+      <c r="A503" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B503" s="7">
-        <v>43712.625</v>
+        <v>43712.618055555555</v>
       </c>
       <c r="C503" s="7">
-        <v>43712.673611111109</v>
+        <v>43712.701388888891</v>
       </c>
       <c r="D503" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F503" s="6" t="s">
+      <c r="F503" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A504" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B504" s="7">
+        <v>43611.392361111109</v>
+      </c>
+      <c r="C504" s="7">
+        <v>43611.517361111109</v>
+      </c>
+      <c r="D504" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E504" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F504" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A505" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B505" s="7">
+        <v>43611.875</v>
+      </c>
+      <c r="C505" s="7">
+        <v>43612.208333333336</v>
+      </c>
+      <c r="D505" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E505" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F505" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B506" s="7">
+        <v>43712.611111111109</v>
+      </c>
+      <c r="C506" s="7">
+        <v>43712.75</v>
+      </c>
+      <c r="D506" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E506" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F506" t="s">
         <v>65</v>
       </c>
     </row>
@@ -10785,7 +10915,7 @@
   <autoFilter ref="A1:F503">
     <filterColumn colId="0">
       <filters>
-        <filter val="SLR-045"/>
+        <filter val="SDR-780"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -10805,8 +10935,8 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10825,7 +10955,7 @@
         <v>52</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10840,7 +10970,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>63</v>
@@ -10865,7 +10995,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>63</v>
@@ -10883,7 +11013,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>63</v>
@@ -10901,7 +11031,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>63</v>
@@ -10926,7 +11056,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>63</v>
@@ -10937,7 +11067,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C14" s="29" t="s">
         <v>63</v>
@@ -10948,7 +11078,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>63</v>
@@ -10966,7 +11096,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C17" s="29" t="s">
         <v>63</v>
@@ -10991,7 +11121,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C20" s="29" t="s">
         <v>63</v>
@@ -11078,22 +11208,30 @@
       <c r="A32" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="B32" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
         <v>44</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C34" s="29" t="s">
         <v>65</v>
@@ -11104,7 +11242,7 @@
         <v>45</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>65</v>
@@ -11115,7 +11253,7 @@
         <v>46</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>65</v>
@@ -11126,7 +11264,7 @@
         <v>18</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>65</v>
@@ -11137,7 +11275,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>65</v>
@@ -11148,7 +11286,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>65</v>
@@ -11159,7 +11297,7 @@
         <v>20</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>65</v>
@@ -11170,7 +11308,7 @@
         <v>25</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>65</v>

</xml_diff>